<commit_message>
General updates, and powerlimiting to stay under 80kw
</commit_message>
<xml_diff>
--- a/FSAE Car.xlsx
+++ b/FSAE Car.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Isaac\Documents\Lap Simulations\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80699B4A-4722-4894-BD01-0A7C339F90B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{939CCC02-56B3-402A-87FE-E901F2EEB710}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2846" yWindow="883" windowWidth="29494" windowHeight="11923" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25800" windowHeight="21000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Info" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="101">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="102">
   <si>
     <t>General</t>
   </si>
@@ -325,12 +325,6 @@
     <t>Recommended value:  4.72E+07 for petrol</t>
   </si>
   <si>
-    <t>Recommended value:  0.98 for spur/helical gears</t>
-  </si>
-  <si>
-    <t>Recommended value:  0.90 for bevel gears</t>
-  </si>
-  <si>
     <t>Generiv F1 car.</t>
   </si>
   <si>
@@ -338,6 +332,15 @@
   </si>
   <si>
     <t>FSAE Car</t>
+  </si>
+  <si>
+    <t>Inverter Losses</t>
+  </si>
+  <si>
+    <t>Motor Losses</t>
+  </si>
+  <si>
+    <t>Drivetrain Losses</t>
   </si>
 </sst>
 </file>
@@ -1019,20 +1022,20 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E52"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="C44" sqref="C44"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="13.69140625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="30.3828125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="12.15234375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.53515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="81.15234375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="13.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="30.42578125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="81.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="22" t="s">
         <v>45</v>
       </c>
@@ -1049,7 +1052,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="32" t="s">
         <v>0</v>
       </c>
@@ -1057,16 +1060,16 @@
         <v>1</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="D2" s="9" t="s">
         <v>38</v>
       </c>
       <c r="E2" s="10" t="s">
-        <v>98</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="33"/>
       <c r="B3" s="11" t="s">
         <v>2</v>
@@ -1079,7 +1082,7 @@
       </c>
       <c r="E3" s="14"/>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="32" t="s">
         <v>12</v>
       </c>
@@ -1087,14 +1090,14 @@
         <v>3</v>
       </c>
       <c r="C4" s="8">
-        <v>250</v>
+        <v>220</v>
       </c>
       <c r="D4" s="9" t="s">
         <v>6</v>
       </c>
       <c r="E4" s="10"/>
     </row>
-    <row r="5" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="33"/>
       <c r="B5" s="11" t="s">
         <v>4</v>
@@ -1107,7 +1110,7 @@
       </c>
       <c r="E5" s="14"/>
     </row>
-    <row r="6" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A6" s="15" t="s">
         <v>10</v>
       </c>
@@ -1122,7 +1125,7 @@
       </c>
       <c r="E6" s="19"/>
     </row>
-    <row r="7" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="15" t="s">
         <v>11</v>
       </c>
@@ -1139,7 +1142,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" s="32" t="s">
         <v>14</v>
       </c>
@@ -1156,7 +1159,7 @@
         <v>82</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="34"/>
       <c r="B9" s="1" t="s">
         <v>74</v>
@@ -1171,7 +1174,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="34"/>
       <c r="B10" s="1" t="s">
         <v>21</v>
@@ -1184,7 +1187,7 @@
       </c>
       <c r="E10" s="20"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="34"/>
       <c r="B11" s="1" t="s">
         <v>22</v>
@@ -1197,7 +1200,7 @@
       </c>
       <c r="E11" s="20"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="34"/>
       <c r="B12" s="1" t="s">
         <v>72</v>
@@ -1210,7 +1213,7 @@
       </c>
       <c r="E12" s="20"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" s="34"/>
       <c r="B13" s="1" t="s">
         <v>17</v>
@@ -1223,7 +1226,7 @@
       </c>
       <c r="E13" s="20"/>
     </row>
-    <row r="14" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="33"/>
       <c r="B14" s="11" t="s">
         <v>23</v>
@@ -1238,7 +1241,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" s="32" t="s">
         <v>20</v>
       </c>
@@ -1255,7 +1258,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="34"/>
       <c r="B16" s="1" t="s">
         <v>25</v>
@@ -1270,7 +1273,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="34"/>
       <c r="B17" s="1" t="s">
         <v>78</v>
@@ -1285,7 +1288,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="34"/>
       <c r="B18" s="1" t="s">
         <v>26</v>
@@ -1300,7 +1303,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="34"/>
       <c r="B19" s="1" t="s">
         <v>27</v>
@@ -1315,7 +1318,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="34"/>
       <c r="B20" s="1" t="s">
         <v>28</v>
@@ -1330,7 +1333,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="21" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A21" s="33"/>
       <c r="B21" s="11" t="s">
         <v>29</v>
@@ -1345,7 +1348,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="32" t="s">
         <v>30</v>
       </c>
@@ -1360,13 +1363,13 @@
       </c>
       <c r="E22" s="10"/>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="34"/>
       <c r="B23" s="1" t="s">
         <v>31</v>
       </c>
       <c r="C23" s="3">
-        <v>266.7</v>
+        <v>260.35000000000002</v>
       </c>
       <c r="D23" s="2" t="s">
         <v>8</v>
@@ -1375,7 +1378,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="34"/>
       <c r="B24" s="1" t="s">
         <v>36</v>
@@ -1390,7 +1393,7 @@
         <v>89</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="34"/>
       <c r="B25" s="1" t="s">
         <v>32</v>
@@ -1405,13 +1408,13 @@
         <v>90</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="34"/>
       <c r="B26" s="1" t="s">
         <v>33</v>
       </c>
       <c r="C26" s="3">
-        <v>250</v>
+        <v>66</v>
       </c>
       <c r="D26" s="2" t="s">
         <v>6</v>
@@ -1420,7 +1423,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="34"/>
       <c r="B27" s="1" t="s">
         <v>34</v>
@@ -1435,7 +1438,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="34"/>
       <c r="B28" s="1" t="s">
         <v>39</v>
@@ -1450,13 +1453,13 @@
         <v>90</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="34"/>
       <c r="B29" s="1" t="s">
         <v>40</v>
       </c>
       <c r="C29" s="3">
-        <v>250</v>
+        <v>66</v>
       </c>
       <c r="D29" s="2" t="s">
         <v>6</v>
@@ -1465,7 +1468,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="34"/>
       <c r="B30" s="1" t="s">
         <v>41</v>
@@ -1480,7 +1483,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="34"/>
       <c r="B31" s="1" t="s">
         <v>42</v>
@@ -1495,7 +1498,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="32" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="32" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A32" s="33"/>
       <c r="B32" s="11" t="s">
         <v>43</v>
@@ -1510,7 +1513,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="32" t="s">
         <v>50</v>
       </c>
@@ -1525,7 +1528,7 @@
       </c>
       <c r="E33" s="10"/>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="34"/>
       <c r="B34" s="1" t="s">
         <v>52</v>
@@ -1540,7 +1543,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="35" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A35" s="33"/>
       <c r="B35" s="11" t="s">
         <v>53</v>
@@ -1555,7 +1558,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="29" t="s">
         <v>55</v>
       </c>
@@ -1570,7 +1573,7 @@
       </c>
       <c r="E36" s="10"/>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="30"/>
       <c r="B37" s="4" t="s">
         <v>79</v>
@@ -1585,22 +1588,22 @@
         <v>81</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="30"/>
       <c r="B38" s="4" t="s">
         <v>75</v>
       </c>
       <c r="C38" s="5">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>38</v>
       </c>
       <c r="E38" s="28" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.4">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="30"/>
       <c r="B39" s="4" t="s">
         <v>76</v>
@@ -1612,25 +1615,25 @@
         <v>38</v>
       </c>
       <c r="E39" s="28" t="s">
-        <v>97</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.4">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="30"/>
       <c r="B40" s="4" t="s">
         <v>77</v>
       </c>
       <c r="C40" s="5">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>38</v>
       </c>
       <c r="E40" s="28" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.4">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="30"/>
       <c r="B41" s="1" t="s">
         <v>60</v>
@@ -1642,10 +1645,10 @@
         <v>38</v>
       </c>
       <c r="E41" s="20" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="42" spans="1:5" x14ac:dyDescent="0.4">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="30"/>
       <c r="B42" s="1" t="s">
         <v>61</v>
@@ -1658,20 +1661,20 @@
       </c>
       <c r="E42" s="20"/>
     </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="30"/>
       <c r="B43" s="26" t="s">
         <v>62</v>
       </c>
       <c r="C43" s="3">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="D43" s="2" t="s">
         <v>38</v>
       </c>
       <c r="E43" s="20"/>
     </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="30"/>
       <c r="B44" s="26" t="s">
         <v>63</v>
@@ -1682,7 +1685,7 @@
       </c>
       <c r="E44" s="20"/>
     </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="30"/>
       <c r="B45" s="26" t="s">
         <v>64</v>
@@ -1693,7 +1696,7 @@
       </c>
       <c r="E45" s="20"/>
     </row>
-    <row r="46" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="30"/>
       <c r="B46" s="26" t="s">
         <v>65</v>
@@ -1704,7 +1707,7 @@
       </c>
       <c r="E46" s="20"/>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="30"/>
       <c r="B47" s="26" t="s">
         <v>66</v>
@@ -1715,7 +1718,7 @@
       </c>
       <c r="E47" s="20"/>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="30"/>
       <c r="B48" s="26" t="s">
         <v>67</v>
@@ -1726,7 +1729,7 @@
       </c>
       <c r="E48" s="20"/>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="30"/>
       <c r="B49" s="26" t="s">
         <v>68</v>
@@ -1737,7 +1740,7 @@
       </c>
       <c r="E49" s="20"/>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="30"/>
       <c r="B50" s="26" t="s">
         <v>69</v>
@@ -1748,7 +1751,7 @@
       </c>
       <c r="E50" s="20"/>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="30"/>
       <c r="B51" s="26" t="s">
         <v>70</v>
@@ -1759,7 +1762,7 @@
       </c>
       <c r="E51" s="20"/>
     </row>
-    <row r="52" spans="1:5" ht="15" thickBot="1" x14ac:dyDescent="0.45">
+    <row r="52" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A52" s="31"/>
       <c r="B52" s="27" t="s">
         <v>71</v>
@@ -1790,16 +1793,16 @@
   <dimension ref="A1:B38"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+      <selection activeCell="F11" sqref="F11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="20" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>15</v>
       </c>
@@ -1807,7 +1810,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1E-3</v>
       </c>
@@ -1815,7 +1818,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>176.429134</v>
       </c>
@@ -1823,7 +1826,7 @@
         <v>94.452333909999993</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>525.71596209999996</v>
       </c>
@@ -1831,7 +1834,7 @@
         <v>95.101223950000005</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>875.00279020000005</v>
       </c>
@@ -1839,7 +1842,7 @@
         <v>94.475929910000005</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1224.289618</v>
       </c>
@@ -1847,7 +1850,7 @@
         <v>93.579281839999993</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1573.576446</v>
       </c>
@@ -1855,7 +1858,7 @@
         <v>93.0247758</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1922.863274</v>
       </c>
@@ -1863,7 +1866,7 @@
         <v>92.517461769999997</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>2272.1501029999999</v>
       </c>
@@ -1871,7 +1874,7 @@
         <v>92.210713740000003</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2621.4369310000002</v>
       </c>
@@ -1879,7 +1882,7 @@
         <v>91.656207699999996</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>2970.723759</v>
       </c>
@@ -1887,7 +1890,7 @@
         <v>91.16069167000002</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3320.0105870000002</v>
       </c>
@@ -1895,7 +1898,7 @@
         <v>90.488205620000002</v>
       </c>
     </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>3669.297415</v>
       </c>
@@ -1903,7 +1906,7 @@
         <v>90.051679590000006</v>
       </c>
     </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>4018.5842429999998</v>
       </c>
@@ -1911,7 +1914,7 @@
         <v>89.957295579999993</v>
       </c>
     </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>4367.8710709999996</v>
       </c>
@@ -1919,7 +1922,7 @@
         <v>89.390991540000002</v>
       </c>
     </row>
-    <row r="16" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>4717.1578989999998</v>
       </c>
@@ -1927,7 +1930,7 @@
         <v>88.671313490000003</v>
       </c>
     </row>
-    <row r="17" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>5066.4447270000001</v>
       </c>
@@ -1935,7 +1938,7 @@
         <v>87.975231440000002</v>
       </c>
     </row>
-    <row r="18" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>5415.7315550000003</v>
       </c>
@@ -1943,7 +1946,7 @@
         <v>87.267351379999994</v>
       </c>
     </row>
-    <row r="19" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>5765.0183829999996</v>
       </c>
@@ -1951,7 +1954,7 @@
         <v>86.524077329999997</v>
       </c>
     </row>
-    <row r="20" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>6114.3052109999999</v>
       </c>
@@ -1959,7 +1962,7 @@
         <v>85.379671250000001</v>
       </c>
     </row>
-    <row r="21" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>6463.5920400000005</v>
       </c>
@@ -1967,7 +1970,7 @@
         <v>83.315021099999996</v>
       </c>
     </row>
-    <row r="22" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>6812.8788679999998</v>
       </c>
@@ -1975,7 +1978,7 @@
         <v>81.226774950000006</v>
       </c>
     </row>
-    <row r="23" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>7162.165696</v>
       </c>
@@ -1983,7 +1986,7 @@
         <v>79.126730800000004</v>
       </c>
     </row>
-    <row r="24" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>7511.4525240000003</v>
       </c>
@@ -1991,7 +1994,7 @@
         <v>77.05028265</v>
       </c>
     </row>
-    <row r="25" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>7860.7393519999996</v>
       </c>
@@ -1999,7 +2002,7 @@
         <v>74.926642490000006</v>
       </c>
     </row>
-    <row r="26" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>8210.0261800000007</v>
       </c>
@@ -2007,7 +2010,7 @@
         <v>72.543446320000001</v>
       </c>
     </row>
-    <row r="27" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>8559.3130079999992</v>
       </c>
@@ -2015,7 +2018,7 @@
         <v>69.877098129999993</v>
       </c>
     </row>
-    <row r="28" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>8908.5998359999994</v>
       </c>
@@ -2023,7 +2026,7 @@
         <v>67.257941939999995</v>
       </c>
     </row>
-    <row r="29" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>9257.8866639999997</v>
       </c>
@@ -2031,7 +2034,7 @@
         <v>64.615189749999999</v>
       </c>
     </row>
-    <row r="30" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>9607.1734919999999</v>
       </c>
@@ -2039,7 +2042,7 @@
         <v>61.96063955000001</v>
       </c>
     </row>
-    <row r="31" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>9956.4603200000001</v>
       </c>
@@ -2047,7 +2050,7 @@
         <v>59.341483359999998</v>
       </c>
     </row>
-    <row r="32" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>10305.747149999999</v>
       </c>
@@ -2055,7 +2058,7 @@
         <v>57.135257199999998</v>
       </c>
     </row>
-    <row r="33" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>10655.03398</v>
       </c>
@@ -2063,7 +2066,7 @@
         <v>54.95262704999999</v>
       </c>
     </row>
-    <row r="34" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>11004.3208</v>
       </c>
@@ -2071,7 +2074,7 @@
         <v>52.864380889999993</v>
       </c>
     </row>
-    <row r="35" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>11353.60763</v>
       </c>
@@ -2079,7 +2082,7 @@
         <v>50.89411475</v>
       </c>
     </row>
-    <row r="36" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>11702.89446</v>
       </c>
@@ -2087,7 +2090,7 @@
         <v>48.782272599999999</v>
       </c>
     </row>
-    <row r="37" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>12052.18129</v>
       </c>
@@ -2095,7 +2098,7 @@
         <v>46.906390459999997</v>
       </c>
     </row>
-    <row r="38" spans="1:2" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>12401.46812</v>
       </c>

</xml_diff>